<commit_message>
Adding update and UbiComp changes
</commit_message>
<xml_diff>
--- a/conferences/UbiComp 2016/UbiComp 2016.xlsx
+++ b/conferences/UbiComp 2016/UbiComp 2016.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mark.rucker\My Projects\mr2an\conferences\UbiComp 2016\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mark\My Projects\mr2an\conferences\UbiComp 2016\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -28,6 +28,7 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Mark Rucker</author>
+    <author>Mark</author>
   </authors>
   <commentList>
     <comment ref="B15" authorId="0" shapeId="0">
@@ -295,12 +296,36 @@
         </r>
       </text>
     </comment>
+    <comment ref="B100" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Mark:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Possibly interesting but the author's don't seem to share my interest and aren't in America. I wasn't able to find an abstract to *know* I'm interested.</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1717" uniqueCount="1238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1728" uniqueCount="1244">
   <si>
     <t>Title</t>
   </si>
@@ -4014,6 +4039,24 @@
   </si>
   <si>
     <t>Mobile Health, UC, Machine Learning</t>
+  </si>
+  <si>
+    <t>Make Abilities Group</t>
+  </si>
+  <si>
+    <t>Environmental Sustainability, Dynamic Surveys, Machine Learning</t>
+  </si>
+  <si>
+    <t>Maurice Falk University Professor</t>
+  </si>
+  <si>
+    <t>Lots, Statistics, Surveys</t>
+  </si>
+  <si>
+    <t>Associate Professor</t>
+  </si>
+  <si>
+    <t>HCI, Usability, Tech Tools for Creating</t>
   </si>
 </sst>
 </file>
@@ -4127,7 +4170,7 @@
     </filterColumn>
     <filterColumn colId="2">
       <filters>
-        <filter val="14:00"/>
+        <filter val="16:00"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -4431,7 +4474,7 @@
   <dimension ref="B2:I137"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E100" sqref="E100"/>
+      <selection activeCell="B113" sqref="B113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4440,7 +4483,7 @@
     <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="79.7109375" customWidth="1"/>
-    <col min="6" max="6" width="120.28515625" customWidth="1"/>
+    <col min="6" max="6" width="76.42578125" customWidth="1"/>
     <col min="7" max="7" width="43.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="85.28515625" customWidth="1"/>
@@ -6638,7 +6681,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="97" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B97" t="b">
         <v>1</v>
       </c>
@@ -6648,7 +6691,7 @@
       <c r="D97" s="2">
         <v>0.58333333333333337</v>
       </c>
-      <c r="E97" t="s">
+      <c r="E97" s="3" t="s">
         <v>221</v>
       </c>
       <c r="F97" t="s">
@@ -6661,9 +6704,9 @@
         <v>56</v>
       </c>
     </row>
-    <row r="98" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B98" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C98" s="1">
         <v>42629</v>
@@ -6684,7 +6727,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="99" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B99" t="b">
         <v>0</v>
       </c>
@@ -6707,9 +6750,9 @@
         <v>56</v>
       </c>
     </row>
-    <row r="100" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B100" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C100" s="1">
         <v>42629</v>
@@ -6730,7 +6773,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="101" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B101" t="b">
         <v>1</v>
       </c>
@@ -6740,7 +6783,7 @@
       <c r="D101" s="2">
         <v>0.58333333333333304</v>
       </c>
-      <c r="E101" t="s">
+      <c r="E101" s="3" t="s">
         <v>229</v>
       </c>
       <c r="F101" t="s">
@@ -6753,7 +6796,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="102" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="102" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B102" t="b">
         <v>1</v>
       </c>
@@ -6776,7 +6819,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="103" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B103" t="b">
         <v>0</v>
       </c>
@@ -6799,7 +6842,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="104" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="104" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B104" t="b">
         <v>0</v>
       </c>
@@ -6822,9 +6865,9 @@
         <v>56</v>
       </c>
     </row>
-    <row r="105" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="105" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B105" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C105" s="1">
         <v>42629</v>
@@ -6845,7 +6888,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="106" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="106" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B106" t="b">
         <v>0</v>
       </c>
@@ -6868,9 +6911,9 @@
         <v>56</v>
       </c>
     </row>
-    <row r="107" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="107" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B107" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C107" s="1">
         <v>42629</v>
@@ -6891,7 +6934,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="108" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="108" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B108" t="b">
         <v>1</v>
       </c>
@@ -6914,9 +6957,9 @@
         <v>56</v>
       </c>
     </row>
-    <row r="109" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B109" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C109" s="1">
         <v>42629</v>
@@ -6937,7 +6980,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="110" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B110" t="b">
         <v>0</v>
       </c>
@@ -6960,7 +7003,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="111" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B111" t="b">
         <v>0</v>
       </c>
@@ -6983,9 +7026,9 @@
         <v>56</v>
       </c>
     </row>
-    <row r="112" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B112" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C112" s="1">
         <v>42629</v>
@@ -7006,7 +7049,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="113" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B113" t="b">
         <v>1</v>
       </c>
@@ -7029,7 +7072,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="114" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B114" t="b">
         <v>1</v>
       </c>
@@ -7052,7 +7095,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="115" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B115" t="b">
         <v>0</v>
       </c>
@@ -7075,7 +7118,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="116" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B116" t="b">
         <v>0</v>
       </c>
@@ -7098,7 +7141,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="117" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B117" t="b">
         <v>1</v>
       </c>
@@ -7121,7 +7164,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="118" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B118" t="b">
         <v>1</v>
       </c>
@@ -7144,7 +7187,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="119" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B119" t="b">
         <v>1</v>
       </c>
@@ -7167,7 +7210,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="120" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B120" s="2" t="b">
         <v>0</v>
       </c>
@@ -7216,11 +7259,13 @@
     <hyperlink ref="E77" r:id="rId6"/>
     <hyperlink ref="E86" r:id="rId7"/>
     <hyperlink ref="E84" r:id="rId8"/>
+    <hyperlink ref="E101" r:id="rId9"/>
+    <hyperlink ref="E97" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId9"/>
+  <legacyDrawing r:id="rId11"/>
   <tableParts count="1">
-    <tablePart r:id="rId10"/>
+    <tablePart r:id="rId12"/>
   </tableParts>
 </worksheet>
 </file>
@@ -7229,8 +7274,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:I530"/>
   <sheetViews>
-    <sheetView topLeftCell="A152" workbookViewId="0">
-      <selection activeCell="F172" sqref="F172"/>
+    <sheetView topLeftCell="D186" workbookViewId="0">
+      <selection activeCell="G197" sqref="G197"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9000,6 +9045,18 @@
       <c r="D197" t="s">
         <v>1023</v>
       </c>
+      <c r="E197" t="s">
+        <v>1242</v>
+      </c>
+      <c r="F197" t="s">
+        <v>1201</v>
+      </c>
+      <c r="G197" t="s">
+        <v>1238</v>
+      </c>
+      <c r="H197" t="s">
+        <v>1243</v>
+      </c>
     </row>
     <row r="198" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B198" t="s">
@@ -9375,7 +9432,7 @@
         <v>1069</v>
       </c>
     </row>
-    <row r="241" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="241" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B241" t="s">
         <v>447</v>
       </c>
@@ -9383,7 +9440,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="242" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="242" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B242" t="s">
         <v>657</v>
       </c>
@@ -9391,7 +9448,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="243" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="243" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B243" t="s">
         <v>383</v>
       </c>
@@ -9399,7 +9456,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="244" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="244" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B244" t="s">
         <v>937</v>
       </c>
@@ -9407,15 +9464,27 @@
         <v>938</v>
       </c>
     </row>
-    <row r="245" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="245" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B245" t="s">
         <v>1019</v>
       </c>
       <c r="D245" t="s">
         <v>1020</v>
       </c>
-    </row>
-    <row r="246" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E245" t="s">
+        <v>1192</v>
+      </c>
+      <c r="F245" t="s">
+        <v>1201</v>
+      </c>
+      <c r="G245" t="s">
+        <v>1238</v>
+      </c>
+      <c r="H245" t="s">
+        <v>1239</v>
+      </c>
+    </row>
+    <row r="246" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B246" t="s">
         <v>616</v>
       </c>
@@ -9423,7 +9492,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="247" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="247" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B247" t="s">
         <v>1041</v>
       </c>
@@ -9431,7 +9500,7 @@
         <v>1042</v>
       </c>
     </row>
-    <row r="248" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="248" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B248" t="s">
         <v>743</v>
       </c>
@@ -9439,7 +9508,7 @@
         <v>744</v>
       </c>
     </row>
-    <row r="249" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="249" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B249" t="s">
         <v>652</v>
       </c>
@@ -9447,7 +9516,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="250" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="250" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B250" t="s">
         <v>819</v>
       </c>
@@ -9455,7 +9524,7 @@
         <v>820</v>
       </c>
     </row>
-    <row r="251" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="251" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B251" t="s">
         <v>572</v>
       </c>
@@ -9463,7 +9532,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="252" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="252" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B252" t="s">
         <v>428</v>
       </c>
@@ -9471,7 +9540,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="253" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="253" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B253" t="s">
         <v>1145</v>
       </c>
@@ -9479,7 +9548,7 @@
         <v>852</v>
       </c>
     </row>
-    <row r="254" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="254" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B254" t="s">
         <v>656</v>
       </c>
@@ -9487,7 +9556,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="255" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="255" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B255" t="s">
         <v>581</v>
       </c>
@@ -9498,7 +9567,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="256" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="256" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B256" t="s">
         <v>581</v>
       </c>
@@ -11000,6 +11069,15 @@
       </c>
       <c r="D413" t="s">
         <v>1022</v>
+      </c>
+      <c r="E413" t="s">
+        <v>1240</v>
+      </c>
+      <c r="F413" t="s">
+        <v>1201</v>
+      </c>
+      <c r="H413" t="s">
+        <v>1241</v>
       </c>
     </row>
     <row r="414" spans="2:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
One more UbiComp article
</commit_message>
<xml_diff>
--- a/conferences/UbiComp 2016/UbiComp 2016.xlsx
+++ b/conferences/UbiComp 2016/UbiComp 2016.xlsx
@@ -320,12 +320,60 @@
         </r>
       </text>
     </comment>
+    <comment ref="B113" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Mark:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+They have connections with UVA!!!</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B114" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Mark:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+I'm not sure if I'm interested in the authors. They don't seem fully professionally developed. On the other hand maybe that makes them perfect for me to try and connect with.</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1728" uniqueCount="1244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1745" uniqueCount="1252">
   <si>
     <t>Title</t>
   </si>
@@ -4057,6 +4105,30 @@
   </si>
   <si>
     <t>HCI, Usability, Tech Tools for Creating</t>
+  </si>
+  <si>
+    <t>University of California, Merced</t>
+  </si>
+  <si>
+    <t>ANDES Lab</t>
+  </si>
+  <si>
+    <t>University of Michigan</t>
+  </si>
+  <si>
+    <t>She has partnered with UVA CS department for recommender system research</t>
+  </si>
+  <si>
+    <t>HCI Sustainability, HCI Usability</t>
+  </si>
+  <si>
+    <t>Ohio State University</t>
+  </si>
+  <si>
+    <t>Mobile Smart Networking Lab</t>
+  </si>
+  <si>
+    <t>UNIST</t>
   </si>
 </sst>
 </file>
@@ -4163,14 +4235,9 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B2:I120" totalsRowShown="0">
   <autoFilter ref="B2:I120">
-    <filterColumn colId="1">
+    <filterColumn colId="0">
       <filters>
-        <dateGroupItem year="2016" month="9" day="16" dateTimeGrouping="day"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="2">
-      <filters>
-        <filter val="16:00"/>
+        <filter val="TRUE"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -4473,8 +4540,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:I137"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B113" sqref="B113"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4539,7 +4606,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="2:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4" t="b">
         <v>1</v>
       </c>
@@ -4864,7 +4931,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="18" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18" t="b">
         <v>1</v>
       </c>
@@ -5324,7 +5391,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="38" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B38" t="b">
         <v>1</v>
       </c>
@@ -5395,7 +5462,7 @@
     </row>
     <row r="41" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B41" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C41" s="1">
         <v>42627</v>
@@ -5508,7 +5575,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="46" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B46" t="b">
         <v>1</v>
       </c>
@@ -5531,7 +5598,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="47" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B47" t="b">
         <v>1</v>
       </c>
@@ -5577,7 +5644,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="49" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B49" t="b">
         <v>1</v>
       </c>
@@ -5623,7 +5690,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="51" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B51" t="b">
         <v>1</v>
       </c>
@@ -5669,7 +5736,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="53" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B53" t="b">
         <v>1</v>
       </c>
@@ -5692,7 +5759,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="54" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B54" t="b">
         <v>1</v>
       </c>
@@ -5899,7 +5966,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="63" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B63" t="b">
         <v>1</v>
       </c>
@@ -5922,7 +5989,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="64" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B64" t="b">
         <v>1</v>
       </c>
@@ -6175,7 +6242,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="75" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B75" t="b">
         <v>1</v>
       </c>
@@ -6221,7 +6288,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="77" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B77" t="b">
         <v>1</v>
       </c>
@@ -6382,7 +6449,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="84" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B84" t="b">
         <v>1</v>
       </c>
@@ -6428,7 +6495,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="86" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B86" t="b">
         <v>1</v>
       </c>
@@ -6681,7 +6748,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="97" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B97" t="b">
         <v>1</v>
       </c>
@@ -6773,7 +6840,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="101" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B101" t="b">
         <v>1</v>
       </c>
@@ -6796,7 +6863,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="102" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B102" t="b">
         <v>1</v>
       </c>
@@ -6934,7 +7001,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="108" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B108" t="b">
         <v>1</v>
       </c>
@@ -6957,7 +7024,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="109" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="109" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B109" t="b">
         <v>0</v>
       </c>
@@ -6980,7 +7047,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="110" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="110" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B110" t="b">
         <v>0</v>
       </c>
@@ -7003,7 +7070,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="111" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="111" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B111" t="b">
         <v>0</v>
       </c>
@@ -7026,7 +7093,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="112" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="112" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B112" t="b">
         <v>0</v>
       </c>
@@ -7072,9 +7139,9 @@
         <v>56</v>
       </c>
     </row>
-    <row r="114" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="114" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B114" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C114" s="1">
         <v>42629</v>
@@ -7095,7 +7162,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="115" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="115" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B115" t="b">
         <v>0</v>
       </c>
@@ -7118,7 +7185,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="116" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="116" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B116" t="b">
         <v>0</v>
       </c>
@@ -7141,9 +7208,9 @@
         <v>56</v>
       </c>
     </row>
-    <row r="117" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="117" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B117" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C117" s="1">
         <v>42629</v>
@@ -7151,7 +7218,7 @@
       <c r="D117" s="2">
         <v>0.66666666666666696</v>
       </c>
-      <c r="E117" t="s">
+      <c r="E117" s="3" t="s">
         <v>261</v>
       </c>
       <c r="F117" t="s">
@@ -7187,9 +7254,9 @@
         <v>56</v>
       </c>
     </row>
-    <row r="119" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="119" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B119" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C119" s="1">
         <v>42629</v>
@@ -7210,7 +7277,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="120" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="120" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B120" s="2" t="b">
         <v>0</v>
       </c>
@@ -7261,11 +7328,12 @@
     <hyperlink ref="E84" r:id="rId8"/>
     <hyperlink ref="E101" r:id="rId9"/>
     <hyperlink ref="E97" r:id="rId10"/>
+    <hyperlink ref="E117" r:id="rId11"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId11"/>
+  <legacyDrawing r:id="rId12"/>
   <tableParts count="1">
-    <tablePart r:id="rId12"/>
+    <tablePart r:id="rId13"/>
   </tableParts>
 </worksheet>
 </file>
@@ -7274,8 +7342,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:I530"/>
   <sheetViews>
-    <sheetView topLeftCell="D186" workbookViewId="0">
-      <selection activeCell="G197" sqref="G197"/>
+    <sheetView topLeftCell="A242" workbookViewId="0">
+      <selection activeCell="E253" sqref="E253"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7425,6 +7493,18 @@
       <c r="D14" t="s">
         <v>1124</v>
       </c>
+      <c r="E14" t="s">
+        <v>1192</v>
+      </c>
+      <c r="F14" t="s">
+        <v>1244</v>
+      </c>
+      <c r="G14" t="s">
+        <v>1245</v>
+      </c>
+      <c r="H14" t="s">
+        <v>1175</v>
+      </c>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
@@ -8057,6 +8137,18 @@
       <c r="D84" t="s">
         <v>1123</v>
       </c>
+      <c r="E84" t="s">
+        <v>1192</v>
+      </c>
+      <c r="F84" t="s">
+        <v>1244</v>
+      </c>
+      <c r="G84" t="s">
+        <v>1245</v>
+      </c>
+      <c r="H84" t="s">
+        <v>1175</v>
+      </c>
     </row>
     <row r="85" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B85" t="s">
@@ -9149,7 +9241,7 @@
         <v>1055</v>
       </c>
     </row>
-    <row r="209" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="209" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B209" t="s">
         <v>555</v>
       </c>
@@ -9157,7 +9249,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="210" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="210" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B210" t="s">
         <v>403</v>
       </c>
@@ -9165,7 +9257,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="211" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="211" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B211" t="s">
         <v>410</v>
       </c>
@@ -9173,7 +9265,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="212" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="212" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B212" t="s">
         <v>587</v>
       </c>
@@ -9181,7 +9273,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="213" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="213" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B213" t="s">
         <v>686</v>
       </c>
@@ -9189,7 +9281,7 @@
         <v>687</v>
       </c>
     </row>
-    <row r="214" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="214" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B214" t="s">
         <v>507</v>
       </c>
@@ -9197,7 +9289,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="215" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="215" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B215" t="s">
         <v>507</v>
       </c>
@@ -9205,7 +9297,7 @@
         <v>929</v>
       </c>
     </row>
-    <row r="216" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="216" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B216" t="s">
         <v>331</v>
       </c>
@@ -9213,15 +9305,21 @@
         <v>332</v>
       </c>
     </row>
-    <row r="217" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="217" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B217" t="s">
         <v>1144</v>
       </c>
       <c r="D217" t="s">
         <v>852</v>
       </c>
-    </row>
-    <row r="218" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E217" t="s">
+        <v>1195</v>
+      </c>
+      <c r="F217" t="s">
+        <v>1249</v>
+      </c>
+    </row>
+    <row r="218" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B218" t="s">
         <v>320</v>
       </c>
@@ -9232,7 +9330,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="219" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="219" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B219" t="s">
         <v>335</v>
       </c>
@@ -9240,7 +9338,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="220" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="220" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B220" t="s">
         <v>337</v>
       </c>
@@ -9248,7 +9346,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="221" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="221" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B221" t="s">
         <v>675</v>
       </c>
@@ -9256,7 +9354,7 @@
         <v>676</v>
       </c>
     </row>
-    <row r="222" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="222" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B222" t="s">
         <v>1136</v>
       </c>
@@ -9264,7 +9362,7 @@
         <v>1137</v>
       </c>
     </row>
-    <row r="223" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="223" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B223" t="s">
         <v>546</v>
       </c>
@@ -9272,7 +9370,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="224" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="224" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B224" t="s">
         <v>628</v>
       </c>
@@ -9547,6 +9645,15 @@
       <c r="D253" t="s">
         <v>852</v>
       </c>
+      <c r="E253" t="s">
+        <v>1229</v>
+      </c>
+      <c r="F253" t="s">
+        <v>1251</v>
+      </c>
+      <c r="G253" t="s">
+        <v>1250</v>
+      </c>
     </row>
     <row r="254" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B254" t="s">
@@ -10476,6 +10583,18 @@
       </c>
       <c r="D352" t="s">
         <v>323</v>
+      </c>
+      <c r="E352" t="s">
+        <v>1193</v>
+      </c>
+      <c r="F352" t="s">
+        <v>1246</v>
+      </c>
+      <c r="H352" t="s">
+        <v>1248</v>
+      </c>
+      <c r="I352" t="s">
+        <v>1247</v>
       </c>
     </row>
     <row r="353" spans="2:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updats and new Article
</commit_message>
<xml_diff>
--- a/conferences/UbiComp 2016/UbiComp 2016.xlsx
+++ b/conferences/UbiComp 2016/UbiComp 2016.xlsx
@@ -4540,8 +4540,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:I137"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5759,9 +5759,9 @@
         <v>56</v>
       </c>
     </row>
-    <row r="54" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B54" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C54" s="1">
         <v>42628</v>
@@ -5966,9 +5966,9 @@
         <v>56</v>
       </c>
     </row>
-    <row r="63" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B63" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C63" s="1">
         <v>42628</v>
@@ -6288,9 +6288,9 @@
         <v>56</v>
       </c>
     </row>
-    <row r="77" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B77" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C77" s="1">
         <v>42628</v>

</xml_diff>